<commit_message>
Update spatial median splitting.
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -8,26 +8,62 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Kd-tree</t>
   </si>
   <si>
     <t>naïve</t>
   </si>
+  <si>
+    <t>Balanced Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random </t>
+  </si>
+  <si>
+    <t>Query time</t>
+  </si>
+  <si>
+    <t>Depth of the tree</t>
+  </si>
+  <si>
+    <t>N^2 algorithm</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Query Time (Median vs Random for the separating plane)</t>
+  </si>
+  <si>
+    <t>Query time (Kd-tree vs N^2 algorithm)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -55,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -85,6 +122,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Intersection</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Detection Time</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -96,7 +157,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -106,50 +167,54 @@
             </c:strRef>
           </c:tx>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$4:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900</c:v>
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
+              <c:f>Sheet1!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.02</c:v>
                 </c:pt>
@@ -157,7 +222,7 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.02</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.02</c:v>
@@ -166,15 +231,18 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.01</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.02</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.01</c:v>
-                </c:pt>
                 <c:pt idx="8">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.02</c:v>
                 </c:pt>
               </c:numCache>
@@ -187,86 +255,93 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>naïve</c:v>
+                  <c:v>N^2 algorithm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$4:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900</c:v>
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$10</c:f>
+              <c:f>Sheet1!$C$4:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.11</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27</c:v>
+                  <c:v>1.57</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.33</c:v>
+                  <c:v>2.0699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.47</c:v>
+                  <c:v>2.54</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>3.02</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.61</c:v>
+                  <c:v>3.52</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.72</c:v>
+                  <c:v>3.94</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.82</c:v>
+                  <c:v>4.4400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -283,11 +358,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="4931584"/>
-        <c:axId val="4933120"/>
+        <c:axId val="112125824"/>
+        <c:axId val="112128000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="4931584"/>
+        <c:axId val="112125824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -321,7 +396,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4933120"/>
+        <c:crossAx val="112128000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -329,7 +404,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4933120"/>
+        <c:axId val="112128000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -359,7 +434,1351 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4931584"/>
+        <c:crossAx val="112125824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Depth of the tree</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Median</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$39:$A$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$39:$B$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$39:$A$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$39:$C$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="112497792"/>
+        <c:axId val="112499712"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="112497792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># line segments</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="112499712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="112499712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Depth of the</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> tree</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="112497792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Query Time (Median vs Random)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Median</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$22:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$22:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.02</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$22:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$22:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="77224960"/>
+        <c:axId val="77234560"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="77224960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># line segments</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77234560"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="77234560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time [msec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77224960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Intersection</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Detection Time</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kd-tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$4:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$4:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.02</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>naïve</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$4:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$4:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.82</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="42011648"/>
+        <c:axId val="42013824"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="42011648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># line</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> segments</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="42013824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="42013824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time [msec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="42011648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Depth of the tree</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Balanced Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$25:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$25:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$25:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$25:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="40677760"/>
+        <c:axId val="40679680"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="40677760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># line segments</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="40679680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="40679680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Depth of the</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> tree</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="40677760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -385,16 +1804,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>328611</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>166686</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>319086</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>333374</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -408,6 +1827,135 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>328611</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>223836</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>33336</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -703,123 +2251,634 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A2:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>100</v>
-      </c>
-      <c r="B2">
-        <v>0.02</v>
-      </c>
-      <c r="C2">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>200</v>
-      </c>
-      <c r="B3">
-        <v>0.02</v>
-      </c>
-      <c r="C3">
-        <v>0.24</v>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="B4">
         <v>0.02</v>
       </c>
       <c r="C4">
-        <v>0.27</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="B5">
         <v>0.02</v>
       </c>
       <c r="C5">
-        <v>0.33</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>500</v>
+        <v>3000</v>
+      </c>
+      <c r="B6">
+        <v>0.03</v>
+      </c>
+      <c r="C6">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4000</v>
+      </c>
+      <c r="B7">
+        <v>0.02</v>
+      </c>
+      <c r="C7">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5000</v>
+      </c>
+      <c r="B8">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6000</v>
+      </c>
+      <c r="B9">
+        <v>0.02</v>
+      </c>
+      <c r="C9">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7000</v>
+      </c>
+      <c r="B10">
+        <v>0.03</v>
+      </c>
+      <c r="C10">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8000</v>
+      </c>
+      <c r="B11">
+        <v>0.02</v>
+      </c>
+      <c r="C11">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9000</v>
+      </c>
+      <c r="B12">
+        <v>0.03</v>
+      </c>
+      <c r="C12">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10000</v>
+      </c>
+      <c r="B13">
+        <v>0.02</v>
+      </c>
+      <c r="C13">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1000</v>
+      </c>
+      <c r="B22">
+        <v>0.02</v>
+      </c>
+      <c r="C22">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2000</v>
+      </c>
+      <c r="B23">
+        <v>0.02</v>
+      </c>
+      <c r="C23">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3000</v>
+      </c>
+      <c r="B24">
+        <v>0.03</v>
+      </c>
+      <c r="C24">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4000</v>
+      </c>
+      <c r="B25">
+        <v>0.02</v>
+      </c>
+      <c r="C25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5000</v>
+      </c>
+      <c r="B26">
+        <v>0.02</v>
+      </c>
+      <c r="C26">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>6000</v>
+      </c>
+      <c r="B27">
+        <v>0.02</v>
+      </c>
+      <c r="C27">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>7000</v>
+      </c>
+      <c r="B28">
+        <v>0.03</v>
+      </c>
+      <c r="C28">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>8000</v>
+      </c>
+      <c r="B29">
+        <v>0.02</v>
+      </c>
+      <c r="C29">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>9000</v>
+      </c>
+      <c r="B30">
+        <v>0.03</v>
+      </c>
+      <c r="C30">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10000</v>
+      </c>
+      <c r="B31">
+        <v>0.02</v>
+      </c>
+      <c r="C31">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1000</v>
+      </c>
+      <c r="B39">
+        <v>15</v>
+      </c>
+      <c r="C39">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2000</v>
+      </c>
+      <c r="B40">
+        <v>19</v>
+      </c>
+      <c r="C40">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>3000</v>
+      </c>
+      <c r="B41">
+        <v>17</v>
+      </c>
+      <c r="C41">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>4000</v>
+      </c>
+      <c r="B42">
+        <v>20</v>
+      </c>
+      <c r="C42">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>5000</v>
+      </c>
+      <c r="B43">
+        <v>21</v>
+      </c>
+      <c r="C43">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>6000</v>
+      </c>
+      <c r="B44">
+        <v>24</v>
+      </c>
+      <c r="C44">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>7000</v>
+      </c>
+      <c r="B45">
+        <v>24</v>
+      </c>
+      <c r="C45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>8000</v>
+      </c>
+      <c r="B46">
+        <v>23</v>
+      </c>
+      <c r="C46">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>9000</v>
+      </c>
+      <c r="B47">
+        <v>25</v>
+      </c>
+      <c r="C47">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>10000</v>
+      </c>
+      <c r="B48">
+        <v>26</v>
+      </c>
+      <c r="C48">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="121" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>0.02</v>
+      </c>
+      <c r="C4">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>200</v>
+      </c>
+      <c r="B5">
+        <v>0.02</v>
+      </c>
+      <c r="C5">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>300</v>
       </c>
       <c r="B6">
         <v>0.02</v>
       </c>
       <c r="C6">
-        <v>0.47</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="B7">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="C7">
-        <v>0.55000000000000004</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="B8">
         <v>0.02</v>
       </c>
       <c r="C8">
-        <v>0.61</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="B9">
         <v>0.01</v>
       </c>
       <c r="C9">
-        <v>0.72</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="B10">
         <v>0.02</v>
       </c>
       <c r="C10">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>800</v>
+      </c>
+      <c r="B11">
+        <v>0.01</v>
+      </c>
+      <c r="C11">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>900</v>
+      </c>
+      <c r="B12">
+        <v>0.02</v>
+      </c>
+      <c r="C12">
         <v>0.82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>100</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>200</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>300</v>
+      </c>
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>400</v>
+      </c>
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>500</v>
+      </c>
+      <c r="B29">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>600</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>700</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>800</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>900</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="121" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>